<commit_message>
Add table to excel
and make sure dropdowns work
</commit_message>
<xml_diff>
--- a/assessments/FinOps Foundation/assessment.xlsx
+++ b/assessments/FinOps Foundation/assessment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="308">
   <si>
     <t>serial number</t>
   </si>
@@ -925,13 +925,19 @@
     <t>[{'Score': 0, 'Condition': None}]</t>
   </si>
   <si>
-    <t>[{'Score': 10, 'Condition': None}]</t>
+    <t>[{'Score': 1, 'Condition': 'Test for 1'}, {'Score': 5, 'Condition': 'Test for 5'}, {'Score': 10, 'Condition': 'Test for 10'}]</t>
   </si>
   <si>
     <t>0: None</t>
   </si>
   <si>
-    <t>10: None</t>
+    <t>1: Test for 1</t>
+  </si>
+  <si>
+    <t>Sum of Weights</t>
+  </si>
+  <si>
+    <t>Weighted Average Scores</t>
   </si>
 </sst>
 </file>
@@ -1014,6 +1020,16 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="J1:K2" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Sum of Weights"/>
+    <tableColumn id="2" name="Weighted Average Scores"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1312,8 +1328,10 @@
     <col min="3" max="3" width="75.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1340,6 +1358,12 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>306</v>
+      </c>
+      <c r="K1" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -4112,406 +4136,406 @@
     <mergeCell ref="B129:B135"/>
   </mergeCells>
   <dataValidations count="134">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7">
-      <formula1>"10: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F14">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F15">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F17">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F19">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F20">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F21">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F22">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F24">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F25">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F26">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F27">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F28">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F29">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F30">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F31">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F32">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F33">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F34">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F35">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F36">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F37">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F38">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F39">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F40">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F41">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F42">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F43">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F44">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F45">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F46">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F47">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F48">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F49">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F50">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F51">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F52">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F53">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F54">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F55">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F56">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F57">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F58">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F59">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F60">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F61">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F62">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F63">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F64">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F65">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F66">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F67">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F68">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F69">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F70">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F71">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F72">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F73">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F74">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F75">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F76">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F77">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F78">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F79">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F80">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F81">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F82">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F83">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F84">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F85">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F86">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F87">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F88">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F89">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F90">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F91">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F92">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F93">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F94">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F95">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F96">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F97">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F98">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F99">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F100">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F101">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F102">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F103">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F104">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F105">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F106">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F107">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F108">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F109">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F110">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F111">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F112">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F113">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F114">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F115">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F116">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F117">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F118">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F119">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F120">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F121">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F122">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F123">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F124">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F125">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F126">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F127">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F128">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F129">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F130">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F131">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F132">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F133">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F134">
-      <formula1>"0: None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F135">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7">
+      <formula1>"1: Test for 1,5: Test for 5,10: Test for 10"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G12">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G13">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G16">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G17">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G18">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G19">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G20">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G21">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G22">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G23">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G24">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G25">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G26">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G27">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G28">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G29">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G30">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G31">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G32">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G33">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G34">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G35">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G36">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G37">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G38">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G39">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G40">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G41">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G42">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G43">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G44">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G45">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G46">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G47">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G48">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G49">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G50">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G51">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G52">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G53">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G54">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G55">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G56">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G57">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G58">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G59">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G60">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G61">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G62">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G63">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G64">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G65">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G66">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G67">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G68">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G69">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G70">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G71">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G72">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G73">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G74">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G75">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G76">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G77">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G78">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G79">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G80">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G81">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G82">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G83">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G84">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G85">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G86">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G87">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G88">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G89">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G90">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G91">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G92">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G93">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G94">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G95">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G96">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G97">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G98">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G99">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G100">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G101">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G102">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G103">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G104">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G105">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G106">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G107">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G108">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G109">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G110">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G111">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G112">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G113">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G114">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G115">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G116">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G117">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G118">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G119">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G120">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G121">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G122">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G123">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G124">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G125">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G126">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G127">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G128">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G129">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G130">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G131">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G132">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G133">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G134">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G135">
       <formula1>"0: None"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4655,5 +4679,8 @@
   <ignoredErrors>
     <ignoredError sqref="D:D" numberStoredAsText="1"/>
   </ignoredErrors>
+  <tableParts count="1">
+    <tablePart r:id="rId135"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update and adopt subset of actions
For the subset we decided on for the alpha release
</commit_message>
<xml_diff>
--- a/assessments/FinOps Foundation/assessment.xlsx
+++ b/assessments/FinOps Foundation/assessment.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="368">
   <si>
     <t>Sum of Weights</t>
   </si>
@@ -498,7 +498,7 @@
     <t>Create landing zones with access controls, retention, and permissions.</t>
   </si>
   <si>
-    <t>Define data granularity and ingestion frequency; include mandatory metadata.</t>
+    <t>Define data granularity; include mandatory metadata.</t>
   </si>
   <si>
     <t>Document normalization/augmentation rules and owners; version them.</t>
@@ -513,6 +513,9 @@
     <t>Continuously optimize pipelines for timeliness and cost.</t>
   </si>
   <si>
+    <t>Define ingestion frequency; include mandatory metadata.</t>
+  </si>
+  <si>
     <t>Gather personaâ€‘specific requirements; define KPIs/OKRs and glossary.</t>
   </si>
   <si>
@@ -936,16 +939,277 @@
     <t>022</t>
   </si>
   <si>
+    <t>* Define process for reviewing asking for credits from CSPs
+* Define frequency of review, etc.
+10*Ceil(x/2)</t>
+  </si>
+  <si>
+    <t>* Define communication pathways between finops and the business
+* Conduct trainings or create videos
+* Send out period newsletters
+* CI/CD governance
+* Proactive recommendations at deployment
+10*Ceil(x/5)</t>
+  </si>
+  <si>
+    <t>* Process defined for new accounts and resources deployed
+* Train teams on process
+* Automate process
+10*Ceil(x/3)</t>
+  </si>
+  <si>
+    <t>* Define process to address notifications from CSPs
+* Define cadence for review
+* Define exception criteria
+* Define thresholds to change
+* Combine with architecture analysis for SP &amp; RIs
+10*Ceil(x/5)</t>
+  </si>
+  <si>
+    <t>* Process for evaluating spot periodically
+* Tag for date last reviewed
+* New deployments get reviewed beforehand
+* Define requirements for spot
+* Have exception process and expiration date
+10*Ceil(x/5)</t>
+  </si>
+  <si>
+    <t>* Data based on existing patterns
+* Proactive investigations and interviews with teams
+* Proactive self reporting by the business and/or teams
+* 100% catch rate of spikes before they happen
+10*Ceil(x/4)</t>
+  </si>
+  <si>
+    <t>((Forecasted Public Cloud Spend – Actual Public Cloud Spend) / Forecasted Public Cloud Spend)</t>
+  </si>
+  <si>
+    <t>* Periodic review of budget vs forecast
+* Track when projects are forecasted to go over budget
+* Process to request more budget for projects going over
+* RCA to determine cause of budget over run
+10*Ceil(x/4)</t>
+  </si>
+  <si>
+    <t>* Define and follow process for gathering deployment plans from teams
+* Determine timeline for each new project to adjust the forecast during that time
+* Determine how optimizations and lower run rate will impact the forecast on a rolling basis
+10*Ceil(x/3)</t>
+  </si>
+  <si>
+    <t>* Define cost drivers from finance/business
+* Gather metrics on a cadence
+* Set goals/targets
+* Set up forecasting and anomaly detection on units
+10*Ceil(x/4)</t>
+  </si>
+  <si>
+    <t>Increasing Granularity and Visibility
+* Define metadata to track (org, dept, cost center, team, app, etc.)
+* Create the hierarchy for each category of metadata (ex teams per dept, cost centers in an org)
+10*Ceil(x/2)</t>
+  </si>
+  <si>
+    <t>Unallocated Shared CSP Effective Cloud Cost/ Total CSP Effective Cloud Cost</t>
+  </si>
+  <si>
+    <t>Increasing Granularity and Visibility
+* Document as part of tagging strategy and enforcement
+* Teams have visibility into where their resources fit into the hierarchy
+10*Ceil(x/2)</t>
+  </si>
+  <si>
+    <t>Percentage of total costs that are tagged for Each Required Tag</t>
+  </si>
+  <si>
+    <t>Total Effective Costs Associated with Unallocated CSP Cloud Resources During a Period of Time / Total CSP Cloud Costs During a Period of Time</t>
+  </si>
+  <si>
+    <t>Effectiveness/Effort by strategy
+* Manually asking teams to tag resources
+* Remove untagged resources after time threshold
+* Block deployments without proper tags
+* Automatically tag based on CI/CD creator and team
+10*Ceil(x/4)</t>
+  </si>
+  <si>
+    <t>* Manual inspection of spikes
+* Out-of-the-box tool based anomaly alerts
+* Custom simple increase alert calculations
+* Custom alerts per business unit, team, etc.
+* Alerts per unit costs above thresholds
+10*Ceil(x/5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Defined severity tiers
+* Thresholds associated with severity tiers are defined
+* Defined and adhered to response SLAs
+* Published response runbooks
+* Runbook percent successful or completed
+* RCA completed after alerts
+10*Ceil(x/6)
+</t>
+  </si>
+  <si>
+    <t>* Number of detections per time period
+* Number of detections over threshold
+* Time to send notifications to stakeholders
+* Time to validate anomaly
+* Resolution Time/SLA adherence
+* False positive rate
+* Cost Avoidance due to detection
+* Percent anomalies addressed
+10*Ceil(x/8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Define data quality (complete, valid, etc.)
+* Manual quality checks
+* Automated checks (null % on required fields/tags)
+* Response process and triage defined
+* SLAs defined and monitored
+* Integrate with communication and alerting tools
+* Integrate into CI/CD pipelines
+10*Ceil(x/7)
+</t>
+  </si>
+  <si>
+    <t>Not in order, gain points for each task
+* Manual or basic logs
+* Define key metrics (failures, latency, etc.)
+* Static Dashboard updated manually
+* Automated alerts for failures
+* Integrate with communication and alerting tools
+* Define Process &amp; SLAs:RCAs completed for each
+* Tune out false positives
+10*Ceil(x/7)</t>
+  </si>
+  <si>
+    <t>* Manual adjustments to invoices and teams
+* Define Business Rules for sharing discounts, RI/SP, etc.
+* Automate adjustment calculations monthly in arrears
+* Automate mappings into reporting platform for realtime adjustments
+10*Ceil(x/4)</t>
+  </si>
+  <si>
+    <t>* Dashboard for showback
+* Dashboard where teams can dive in to investigate costs
+* Ad-hoc dashboards avaialble to teams
+* Dashboards for key metrics tracking (tagging, waste, etc.)
+10*Ceil(x/4)</t>
+  </si>
+  <si>
     <t>[{'Score': 0, 'Condition': None}]</t>
   </si>
   <si>
-    <t>[{'Score': 1, 'Condition': 'Test for 1'}, {'Score': 5, 'Condition': 'Test for 5'}, {'Score': 10, 'Condition': 'Test for 10'}]</t>
+    <t>[{'Score': 0, 'Condition': 'Not monitored'}, {'Score': 2, 'Condition': 'Reported'}, {'Score': 5, 'Condition': 'Manual remediation'}, {'Score': 10, 'Condition': 'Automated remediation'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No items completed'}, {'Score': 5, 'Condition': '1 item completed'}, {'Score': 10, 'Condition': '2 items completed'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'Not done'}, {'Score': 10, 'Condition': 'Defined'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No rules established'}, {'Score': 10, 'Condition': 'Published policy'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No items completed'}, {'Score': 2, 'Condition': '1 item completed'}, {'Score': 4, 'Condition': '2 items completed'}, {'Score': 6, 'Condition': '3 items completed'}, {'Score': 8, 'Condition': '4 items completed'}, {'Score': 10, 'Condition': '5 items completed'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'Not done'}, {'Score': 10, 'Condition': 'Done and clealy defined'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No items completed'}, {'Score': 4, 'Condition': '1 item completed'}, {'Score': 7, 'Condition': '2 items completed'}, {'Score': 10, 'Condition': '3 items completed'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'Does not exist'}, {'Score': 10, 'Condition': 'Exists'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No documented method'}, {'Score': 10, 'Condition': 'Documented method of assessing modernization efforts'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': '0%'}, {'Score': 1, 'Condition': '10%'}, {'Score': 2, 'Condition': '20%'}, {'Score': 3, 'Condition': '30%'}, {'Score': 4, 'Condition': '40%'}, {'Score': 5, 'Condition': '50%'}, {'Score': 6, 'Condition': '60%'}, {'Score': 7, 'Condition': '70%'}, {'Score': 8, 'Condition': '80%'}, {'Score': 9, 'Condition': '90%'}, {'Score': 10, 'Condition': 'Near 100%'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'Not done'}, {'Score': 10, 'Condition': 'Policy in place and published'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No teardown/shutdown policy'}, {'Score': 3, 'Condition': 'Published policy'}, {'Score': 6, 'Condition': 'Classification tagged or otherwise identifiable'}, {'Score': 10, 'Condition': 'Enforced Policy with tagged/identifiable classifications'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No review of trends'}, {'Score': 3, 'Condition': 'Manual review of trends'}, {'Score': 6, 'Condition': 'Automated trend detection'}, {'Score': 10, 'Condition': 'Manual review and automated trend detection'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No items completed'}, {'Score': 3, 'Condition': '1 item completed'}, {'Score': 5, 'Condition': '2 items completed'}, {'Score': 8, 'Condition': '3 items completed'}, {'Score': 10, 'Condition': '4 items completed'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'None'}, {'Score': 1, 'Condition': 'Annual'}, {'Score': 2, 'Condition': 'Quarterly'}, {'Score': 5, 'Condition': 'Monthly'}, {'Score': 7, 'Condition': 'Bi-Weekly'}, {'Score': 8, 'Condition': 'Weekly'}, {'Score': 10, 'Condition': 'Daily'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No alerting'}, {'Score': 10, 'Condition': 'Alerting exists'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'None'}, {'Score': 10, 'Condition': 'set goal thresholds for kpis and unit costs'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': '0%'}, {'Score': 1, 'Condition': '10%'}, {'Score': 2, 'Condition': '20%'}, {'Score': 3, 'Condition': '30%'}, {'Score': 4, 'Condition': '40%'}, {'Score': 5, 'Condition': '50%'}, {'Score': 6, 'Condition': '60%'}, {'Score': 7, 'Condition': '70%'}, {'Score': 8, 'Condition': '80% '}, {'Score': 9, 'Condition': '90%'}, {'Score': 10, 'Condition': 'Near 100%'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No items completed'}, {'Score': 5, 'Condition': '1 item  completed'}, {'Score': 10, 'Condition': '2 items completed'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No items completed'}, {'Score': 2, 'Condition': '1 item completed'}, {'Score': 4, 'Condition': '2 items completed'}, {'Score': 5, 'Condition': '3 items completed'}, {'Score': 7, 'Condition': '4 items completed'}, {'Score': 9, 'Condition': '5 items completed'}, {'Score': 10, 'Condition': '6 items completed'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No alerting in worflow tools'}, {'Score': 1, 'Condition': 'Alerting in at least one tool'}, {'Score': 3, 'Condition': 'Alerting in some tooling [20%]'}, {'Score': 6, 'Condition': 'Alerting in most tooling [60%]'}, {'Score': 10, 'Condition': 'Alerting in all workflow tools [100%]'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No items completed'}, {'Score': 2, 'Condition': '1 item completed'}, {'Score': 3, 'Condition': '2 items completed'}, {'Score': 4, 'Condition': '3 items completed'}, {'Score': 5, 'Condition': '4 items completed'}, {'Score': 7, 'Condition': '5 items completed'}, {'Score': 8, 'Condition': '6 items completed'}, {'Score': 9, 'Condition': '7 items completed'}, {'Score': 10, 'Condition': '8 items completed'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'Never'}, {'Score': 1, 'Condition': 'Monthly or greater'}, {'Score': 2, 'Condition': 'More than a week'}, {'Score': 3, 'Condition': '7 days'}, {'Score': 4, 'Condition': '5 days'}, {'Score': 6, 'Condition': '2 days'}, {'Score': 8, 'Condition': '1 day'}, {'Score': 10, 'Condition': 'Instant'}]</t>
+  </si>
+  <si>
+    <t>[{'Score': 0, 'Condition': 'No items completed'}, {'Score': 2, 'Condition': '1 items completed'}, {'Score': 3, 'Condition': '2 items completed'}, {'Score': 5, 'Condition': '3 items completed'}, {'Score': 6, 'Condition': '4 items completed'}, {'Score': 8, 'Condition': '5 items completed'}, {'Score': 9, 'Condition': '6 items completed'}, {'Score': 10, 'Condition': '7 items completed'}]</t>
   </si>
   <si>
     <t>0: None</t>
   </si>
   <si>
-    <t>1: Test for 1</t>
+    <t>0: Not monitored</t>
+  </si>
+  <si>
+    <t>0: No items completed</t>
+  </si>
+  <si>
+    <t>0: Not done</t>
+  </si>
+  <si>
+    <t>0: No rules established</t>
+  </si>
+  <si>
+    <t>0: Does not exist</t>
+  </si>
+  <si>
+    <t>0: No documented method</t>
+  </si>
+  <si>
+    <t>0: 0%</t>
+  </si>
+  <si>
+    <t>0: No teardown/shutdown policy</t>
+  </si>
+  <si>
+    <t>0: No review of trends</t>
+  </si>
+  <si>
+    <t>0: No alerting</t>
+  </si>
+  <si>
+    <t>0: No alerting in worflow tools</t>
+  </si>
+  <si>
+    <t>0: Never</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1277,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1084,7 +1351,7 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1609,14 +1876,14 @@
     </row>
     <row r="2" spans="1:54">
       <c r="A2">
-        <f>SUM(Scoring!E2:E135)</f>
+        <f>SUM(Scoring!E2:E136)</f>
         <v>0</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2">
-        <f>SUM(Scoring!H2:H135)/A2</f>
+        <f>SUM(Scoring!H2:H136)/A2</f>
         <v>0</v>
       </c>
       <c r="D2">
@@ -1643,7 +1910,7 @@
         <v>7</v>
       </c>
       <c r="BB4">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1657,7 +1924,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:H136"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1667,55 +1934,56 @@
     <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="75.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="125.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>172</v>
+      <c r="D2" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H2">
         <f>E2*VALUE(LEFT(G2, FIND(":", G2)-1))</f>
@@ -1723,19 +1991,19 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>173</v>
+      <c r="D3" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H3">
         <f>E3*VALUE(LEFT(G3, FIND(":", G3)-1))</f>
@@ -1743,19 +2011,19 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>174</v>
+      <c r="D4" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H4">
         <f>E4*VALUE(LEFT(G4, FIND(":", G4)-1))</f>
@@ -1763,19 +2031,19 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>175</v>
+      <c r="D5" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>308</v>
+        <v>356</v>
       </c>
       <c r="H5">
         <f>E5*VALUE(LEFT(G5, FIND(":", G5)-1))</f>
@@ -1783,19 +2051,19 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>176</v>
+      <c r="D6" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H6">
         <f>E6*VALUE(LEFT(G6, FIND(":", G6)-1))</f>
@@ -1803,21 +2071,21 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>177</v>
+      <c r="D7" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="E7">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>309</v>
+        <v>355</v>
       </c>
       <c r="H7">
         <f>E7*VALUE(LEFT(G7, FIND(":", G7)-1))</f>
@@ -1825,19 +2093,19 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>178</v>
+      <c r="D8" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H8">
         <f>E8*VALUE(LEFT(G8, FIND(":", G8)-1))</f>
@@ -1845,19 +2113,19 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>179</v>
+      <c r="D9" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H9">
         <f>E9*VALUE(LEFT(G9, FIND(":", G9)-1))</f>
@@ -1865,19 +2133,19 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>180</v>
+      <c r="D10" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H10">
         <f>E10*VALUE(LEFT(G10, FIND(":", G10)-1))</f>
@@ -1885,19 +2153,19 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>181</v>
+      <c r="D11" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H11">
         <f>E11*VALUE(LEFT(G11, FIND(":", G11)-1))</f>
@@ -1905,21 +2173,21 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>182</v>
+      <c r="D12" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H12">
         <f>E12*VALUE(LEFT(G12, FIND(":", G12)-1))</f>
@@ -1927,19 +2195,19 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>183</v>
+      <c r="D13" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H13">
         <f>E13*VALUE(LEFT(G13, FIND(":", G13)-1))</f>
@@ -1947,19 +2215,19 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>184</v>
+      <c r="D14" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H14">
         <f>E14*VALUE(LEFT(G14, FIND(":", G14)-1))</f>
@@ -1967,19 +2235,22 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>185</v>
+      <c r="D15" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="G15" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H15">
         <f>E15*VALUE(LEFT(G15, FIND(":", G15)-1))</f>
@@ -1987,19 +2258,19 @@
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>186</v>
+      <c r="D16" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H16">
         <f>E16*VALUE(LEFT(G16, FIND(":", G16)-1))</f>
@@ -2007,21 +2278,21 @@
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>187</v>
+      <c r="D17" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>308</v>
+        <v>358</v>
       </c>
       <c r="H17">
         <f>E17*VALUE(LEFT(G17, FIND(":", G17)-1))</f>
@@ -2029,19 +2300,19 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>188</v>
+      <c r="D18" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H18">
         <f>E18*VALUE(LEFT(G18, FIND(":", G18)-1))</f>
@@ -2049,19 +2320,19 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>189</v>
+      <c r="D19" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H19">
         <f>E19*VALUE(LEFT(G19, FIND(":", G19)-1))</f>
@@ -2069,19 +2340,19 @@
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>190</v>
+      <c r="D20" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H20">
         <f>E20*VALUE(LEFT(G20, FIND(":", G20)-1))</f>
@@ -2089,19 +2360,19 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>191</v>
+      <c r="D21" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H21">
         <f>E21*VALUE(LEFT(G21, FIND(":", G21)-1))</f>
@@ -2109,19 +2380,19 @@
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>192</v>
+      <c r="D22" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H22">
         <f>E22*VALUE(LEFT(G22, FIND(":", G22)-1))</f>
@@ -2129,21 +2400,21 @@
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>193</v>
+      <c r="D23" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H23">
         <f>E23*VALUE(LEFT(G23, FIND(":", G23)-1))</f>
@@ -2151,19 +2422,19 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>194</v>
+      <c r="D24" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>308</v>
+        <v>359</v>
       </c>
       <c r="H24">
         <f>E24*VALUE(LEFT(G24, FIND(":", G24)-1))</f>
@@ -2171,19 +2442,19 @@
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>195</v>
+      <c r="D25" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H25">
         <f>E25*VALUE(LEFT(G25, FIND(":", G25)-1))</f>
@@ -2191,19 +2462,22 @@
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1" t="s">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>196</v>
+      <c r="D26" s="3" t="s">
+        <v>197</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="G26" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H26">
         <f>E26*VALUE(LEFT(G26, FIND(":", G26)-1))</f>
@@ -2211,19 +2485,19 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>197</v>
+      <c r="D27" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H27">
         <f>E27*VALUE(LEFT(G27, FIND(":", G27)-1))</f>
@@ -2231,21 +2505,21 @@
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1" t="s">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>198</v>
+      <c r="D28" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H28">
         <f>E28*VALUE(LEFT(G28, FIND(":", G28)-1))</f>
@@ -2253,19 +2527,19 @@
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>199</v>
+      <c r="D29" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H29">
         <f>E29*VALUE(LEFT(G29, FIND(":", G29)-1))</f>
@@ -2273,19 +2547,19 @@
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>200</v>
+      <c r="D30" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H30">
         <f>E30*VALUE(LEFT(G30, FIND(":", G30)-1))</f>
@@ -2293,19 +2567,19 @@
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>201</v>
+      <c r="D31" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H31">
         <f>E31*VALUE(LEFT(G31, FIND(":", G31)-1))</f>
@@ -2313,19 +2587,19 @@
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>202</v>
+      <c r="D32" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H32">
         <f>E32*VALUE(LEFT(G32, FIND(":", G32)-1))</f>
@@ -2333,19 +2607,19 @@
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>203</v>
+      <c r="D33" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H33">
         <f>E33*VALUE(LEFT(G33, FIND(":", G33)-1))</f>
@@ -2353,21 +2627,21 @@
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1" t="s">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>204</v>
+      <c r="D34" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H34">
         <f>E34*VALUE(LEFT(G34, FIND(":", G34)-1))</f>
@@ -2375,19 +2649,19 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1" t="s">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>205</v>
+      <c r="D35" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H35">
         <f>E35*VALUE(LEFT(G35, FIND(":", G35)-1))</f>
@@ -2395,19 +2669,19 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1" t="s">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>206</v>
+      <c r="D36" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" t="s">
-        <v>308</v>
+        <v>358</v>
       </c>
       <c r="H36">
         <f>E36*VALUE(LEFT(G36, FIND(":", G36)-1))</f>
@@ -2415,19 +2689,19 @@
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1" t="s">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>207</v>
+      <c r="D37" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H37">
         <f>E37*VALUE(LEFT(G37, FIND(":", G37)-1))</f>
@@ -2435,19 +2709,19 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>208</v>
+      <c r="D38" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H38">
         <f>E38*VALUE(LEFT(G38, FIND(":", G38)-1))</f>
@@ -2455,19 +2729,19 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1" t="s">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>209</v>
+      <c r="D39" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>308</v>
+        <v>358</v>
       </c>
       <c r="H39">
         <f>E39*VALUE(LEFT(G39, FIND(":", G39)-1))</f>
@@ -2475,21 +2749,21 @@
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1" t="s">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>210</v>
+      <c r="D40" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H40">
         <f>E40*VALUE(LEFT(G40, FIND(":", G40)-1))</f>
@@ -2497,19 +2771,19 @@
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1" t="s">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>211</v>
+      <c r="D41" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H41">
         <f>E41*VALUE(LEFT(G41, FIND(":", G41)-1))</f>
@@ -2517,19 +2791,22 @@
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1" t="s">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>212</v>
+      <c r="D42" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>309</v>
       </c>
       <c r="G42" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H42">
         <f>E42*VALUE(LEFT(G42, FIND(":", G42)-1))</f>
@@ -2537,19 +2814,19 @@
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1" t="s">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>213</v>
+      <c r="D43" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H43">
         <f>E43*VALUE(LEFT(G43, FIND(":", G43)-1))</f>
@@ -2557,19 +2834,19 @@
       </c>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1" t="s">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>214</v>
+      <c r="D44" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H44">
         <f>E44*VALUE(LEFT(G44, FIND(":", G44)-1))</f>
@@ -2577,19 +2854,19 @@
       </c>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1" t="s">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>215</v>
+      <c r="D45" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H45">
         <f>E45*VALUE(LEFT(G45, FIND(":", G45)-1))</f>
@@ -2597,23 +2874,23 @@
       </c>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>216</v>
+      <c r="D46" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>308</v>
+        <v>360</v>
       </c>
       <c r="H46">
         <f>E46*VALUE(LEFT(G46, FIND(":", G46)-1))</f>
@@ -2621,19 +2898,22 @@
       </c>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1" t="s">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>217</v>
+      <c r="D47" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="G47" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H47">
         <f>E47*VALUE(LEFT(G47, FIND(":", G47)-1))</f>
@@ -2641,19 +2921,19 @@
       </c>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1" t="s">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>218</v>
+      <c r="D48" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" t="s">
-        <v>308</v>
+        <v>361</v>
       </c>
       <c r="H48">
         <f>E48*VALUE(LEFT(G48, FIND(":", G48)-1))</f>
@@ -2661,19 +2941,19 @@
       </c>
     </row>
     <row r="49" spans="1:8">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1" t="s">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>219</v>
+      <c r="D49" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H49">
         <f>E49*VALUE(LEFT(G49, FIND(":", G49)-1))</f>
@@ -2681,19 +2961,19 @@
       </c>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1" t="s">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>220</v>
+      <c r="D50" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H50">
         <f>E50*VALUE(LEFT(G50, FIND(":", G50)-1))</f>
@@ -2701,19 +2981,19 @@
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1" t="s">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>221</v>
+      <c r="D51" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H51">
         <f>E51*VALUE(LEFT(G51, FIND(":", G51)-1))</f>
@@ -2721,21 +3001,21 @@
       </c>
     </row>
     <row r="52" spans="1:8">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1" t="s">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>222</v>
+      <c r="D52" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H52">
         <f>E52*VALUE(LEFT(G52, FIND(":", G52)-1))</f>
@@ -2743,19 +3023,19 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1" t="s">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>223</v>
+      <c r="D53" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="G53" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H53">
         <f>E53*VALUE(LEFT(G53, FIND(":", G53)-1))</f>
@@ -2763,19 +3043,19 @@
       </c>
     </row>
     <row r="54" spans="1:8">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1" t="s">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>224</v>
+      <c r="D54" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="G54" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H54">
         <f>E54*VALUE(LEFT(G54, FIND(":", G54)-1))</f>
@@ -2783,19 +3063,19 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1" t="s">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>225</v>
+      <c r="D55" s="3" t="s">
+        <v>226</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H55">
         <f>E55*VALUE(LEFT(G55, FIND(":", G55)-1))</f>
@@ -2803,19 +3083,19 @@
       </c>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1" t="s">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>226</v>
+      <c r="D56" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H56">
         <f>E56*VALUE(LEFT(G56, FIND(":", G56)-1))</f>
@@ -2823,19 +3103,19 @@
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1" t="s">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>227</v>
+      <c r="D57" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H57">
         <f>E57*VALUE(LEFT(G57, FIND(":", G57)-1))</f>
@@ -2843,21 +3123,21 @@
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1" t="s">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>228</v>
+      <c r="D58" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" t="s">
-        <v>308</v>
+        <v>362</v>
       </c>
       <c r="H58">
         <f>E58*VALUE(LEFT(G58, FIND(":", G58)-1))</f>
@@ -2865,19 +3145,19 @@
       </c>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1" t="s">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>229</v>
+      <c r="D59" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
       <c r="G59" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H59">
         <f>E59*VALUE(LEFT(G59, FIND(":", G59)-1))</f>
@@ -2885,19 +3165,19 @@
       </c>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1" t="s">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>230</v>
+      <c r="D60" s="3" t="s">
+        <v>231</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="G60" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H60">
         <f>E60*VALUE(LEFT(G60, FIND(":", G60)-1))</f>
@@ -2905,19 +3185,19 @@
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1" t="s">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>231</v>
+      <c r="D61" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" t="s">
-        <v>308</v>
+        <v>358</v>
       </c>
       <c r="H61">
         <f>E61*VALUE(LEFT(G61, FIND(":", G61)-1))</f>
@@ -2925,19 +3205,19 @@
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1" t="s">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>232</v>
+      <c r="D62" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="G62" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H62">
         <f>E62*VALUE(LEFT(G62, FIND(":", G62)-1))</f>
@@ -2945,19 +3225,19 @@
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1" t="s">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>233</v>
+      <c r="D63" s="3" t="s">
+        <v>234</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="G63" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H63">
         <f>E63*VALUE(LEFT(G63, FIND(":", G63)-1))</f>
@@ -2965,21 +3245,21 @@
       </c>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1" t="s">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>234</v>
+      <c r="D64" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64" t="s">
-        <v>308</v>
+        <v>358</v>
       </c>
       <c r="H64">
         <f>E64*VALUE(LEFT(G64, FIND(":", G64)-1))</f>
@@ -2987,19 +3267,19 @@
       </c>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1" t="s">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>235</v>
+      <c r="D65" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65" t="s">
-        <v>308</v>
+        <v>358</v>
       </c>
       <c r="H65">
         <f>E65*VALUE(LEFT(G65, FIND(":", G65)-1))</f>
@@ -3007,19 +3287,19 @@
       </c>
     </row>
     <row r="66" spans="1:8">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1" t="s">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>236</v>
+      <c r="D66" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H66">
         <f>E66*VALUE(LEFT(G66, FIND(":", G66)-1))</f>
@@ -3027,19 +3307,19 @@
       </c>
     </row>
     <row r="67" spans="1:8">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1" t="s">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>237</v>
+      <c r="D67" s="3" t="s">
+        <v>238</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="G67" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H67">
         <f>E67*VALUE(LEFT(G67, FIND(":", G67)-1))</f>
@@ -3047,19 +3327,19 @@
       </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1" t="s">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D68" s="2" t="s">
-        <v>238</v>
+      <c r="D68" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="G68" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H68">
         <f>E68*VALUE(LEFT(G68, FIND(":", G68)-1))</f>
@@ -3067,19 +3347,22 @@
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1" t="s">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>239</v>
+      <c r="D69" s="3" t="s">
+        <v>240</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="G69" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H69">
         <f>E69*VALUE(LEFT(G69, FIND(":", G69)-1))</f>
@@ -3087,21 +3370,21 @@
       </c>
     </row>
     <row r="70" spans="1:8">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1" t="s">
+      <c r="A70" s="2"/>
+      <c r="B70" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>240</v>
+      <c r="D70" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H70">
         <f>E70*VALUE(LEFT(G70, FIND(":", G70)-1))</f>
@@ -3109,19 +3392,19 @@
       </c>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1" t="s">
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>241</v>
+      <c r="D71" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71" t="s">
-        <v>308</v>
+        <v>363</v>
       </c>
       <c r="H71">
         <f>E71*VALUE(LEFT(G71, FIND(":", G71)-1))</f>
@@ -3129,19 +3412,19 @@
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1" t="s">
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>242</v>
+      <c r="D72" s="3" t="s">
+        <v>243</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G72" t="s">
-        <v>308</v>
+        <v>362</v>
       </c>
       <c r="H72">
         <f>E72*VALUE(LEFT(G72, FIND(":", G72)-1))</f>
@@ -3149,19 +3432,19 @@
       </c>
     </row>
     <row r="73" spans="1:8">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1" t="s">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>243</v>
+      <c r="D73" s="3" t="s">
+        <v>244</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="G73" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H73">
         <f>E73*VALUE(LEFT(G73, FIND(":", G73)-1))</f>
@@ -3169,19 +3452,19 @@
       </c>
     </row>
     <row r="74" spans="1:8">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1" t="s">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>244</v>
+      <c r="D74" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="G74" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H74">
         <f>E74*VALUE(LEFT(G74, FIND(":", G74)-1))</f>
@@ -3189,19 +3472,19 @@
       </c>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1" t="s">
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D75" s="2" t="s">
-        <v>245</v>
+      <c r="D75" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
       <c r="G75" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H75">
         <f>E75*VALUE(LEFT(G75, FIND(":", G75)-1))</f>
@@ -3209,23 +3492,23 @@
       </c>
     </row>
     <row r="76" spans="1:8">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>246</v>
+      <c r="D76" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="E76">
         <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H76">
         <f>E76*VALUE(LEFT(G76, FIND(":", G76)-1))</f>
@@ -3233,19 +3516,19 @@
       </c>
     </row>
     <row r="77" spans="1:8">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1" t="s">
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>247</v>
+      <c r="D77" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H77">
         <f>E77*VALUE(LEFT(G77, FIND(":", G77)-1))</f>
@@ -3253,19 +3536,19 @@
       </c>
     </row>
     <row r="78" spans="1:8">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1" t="s">
+      <c r="A78" s="2"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D78" s="2" t="s">
-        <v>248</v>
+      <c r="D78" s="3" t="s">
+        <v>249</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
       <c r="G78" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H78">
         <f>E78*VALUE(LEFT(G78, FIND(":", G78)-1))</f>
@@ -3273,19 +3556,19 @@
       </c>
     </row>
     <row r="79" spans="1:8">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1" t="s">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>249</v>
+      <c r="D79" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="E79">
         <v>0</v>
       </c>
       <c r="G79" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H79">
         <f>E79*VALUE(LEFT(G79, FIND(":", G79)-1))</f>
@@ -3293,19 +3576,19 @@
       </c>
     </row>
     <row r="80" spans="1:8">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1" t="s">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>250</v>
+      <c r="D80" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G80" t="s">
-        <v>308</v>
+        <v>364</v>
       </c>
       <c r="H80">
         <f>E80*VALUE(LEFT(G80, FIND(":", G80)-1))</f>
@@ -3313,19 +3596,19 @@
       </c>
     </row>
     <row r="81" spans="1:8">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1" t="s">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>251</v>
+      <c r="D81" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="G81" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H81">
         <f>E81*VALUE(LEFT(G81, FIND(":", G81)-1))</f>
@@ -3333,21 +3616,21 @@
       </c>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1" t="s">
+      <c r="A82" s="2"/>
+      <c r="B82" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>252</v>
+      <c r="D82" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" t="s">
-        <v>308</v>
+        <v>360</v>
       </c>
       <c r="H82">
         <f>E82*VALUE(LEFT(G82, FIND(":", G82)-1))</f>
@@ -3355,19 +3638,19 @@
       </c>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1" t="s">
+      <c r="A83" s="2"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>253</v>
+      <c r="D83" s="3" t="s">
+        <v>254</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G83" t="s">
-        <v>308</v>
+        <v>360</v>
       </c>
       <c r="H83">
         <f>E83*VALUE(LEFT(G83, FIND(":", G83)-1))</f>
@@ -3375,19 +3658,19 @@
       </c>
     </row>
     <row r="84" spans="1:8">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1" t="s">
+      <c r="A84" s="2"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>254</v>
+      <c r="D84" s="3" t="s">
+        <v>255</v>
       </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="G84" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H84">
         <f>E84*VALUE(LEFT(G84, FIND(":", G84)-1))</f>
@@ -3395,19 +3678,19 @@
       </c>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1" t="s">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D85" s="2" t="s">
-        <v>255</v>
+      <c r="D85" s="3" t="s">
+        <v>256</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="G85" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H85">
         <f>E85*VALUE(LEFT(G85, FIND(":", G85)-1))</f>
@@ -3415,19 +3698,19 @@
       </c>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1" t="s">
+      <c r="A86" s="2"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>256</v>
+      <c r="D86" s="3" t="s">
+        <v>257</v>
       </c>
       <c r="E86">
         <v>0</v>
       </c>
       <c r="G86" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H86">
         <f>E86*VALUE(LEFT(G86, FIND(":", G86)-1))</f>
@@ -3435,19 +3718,19 @@
       </c>
     </row>
     <row r="87" spans="1:8">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1" t="s">
+      <c r="A87" s="2"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>257</v>
+      <c r="D87" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="E87">
         <v>0</v>
       </c>
       <c r="G87" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H87">
         <f>E87*VALUE(LEFT(G87, FIND(":", G87)-1))</f>
@@ -3455,21 +3738,21 @@
       </c>
     </row>
     <row r="88" spans="1:8">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1" t="s">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>258</v>
+      <c r="D88" s="3" t="s">
+        <v>259</v>
       </c>
       <c r="E88">
         <v>0</v>
       </c>
       <c r="G88" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H88">
         <f>E88*VALUE(LEFT(G88, FIND(":", G88)-1))</f>
@@ -3477,19 +3760,22 @@
       </c>
     </row>
     <row r="89" spans="1:8">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1" t="s">
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>259</v>
+      <c r="D89" s="3" t="s">
+        <v>260</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="G89" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H89">
         <f>E89*VALUE(LEFT(G89, FIND(":", G89)-1))</f>
@@ -3497,19 +3783,19 @@
       </c>
     </row>
     <row r="90" spans="1:8">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1" t="s">
+      <c r="A90" s="2"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>260</v>
+      <c r="D90" s="3" t="s">
+        <v>261</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H90">
         <f>E90*VALUE(LEFT(G90, FIND(":", G90)-1))</f>
@@ -3517,19 +3803,22 @@
       </c>
     </row>
     <row r="91" spans="1:8">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1" t="s">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D91" s="2" t="s">
-        <v>261</v>
+      <c r="D91" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="G91" t="s">
-        <v>308</v>
+        <v>362</v>
       </c>
       <c r="H91">
         <f>E91*VALUE(LEFT(G91, FIND(":", G91)-1))</f>
@@ -3537,19 +3826,19 @@
       </c>
     </row>
     <row r="92" spans="1:8">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1" t="s">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>262</v>
+      <c r="D92" s="3" t="s">
+        <v>263</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92" t="s">
-        <v>308</v>
+        <v>365</v>
       </c>
       <c r="H92">
         <f>E92*VALUE(LEFT(G92, FIND(":", G92)-1))</f>
@@ -3557,19 +3846,22 @@
       </c>
     </row>
     <row r="93" spans="1:8">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1" t="s">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D93" s="2" t="s">
-        <v>263</v>
+      <c r="D93" s="3" t="s">
+        <v>264</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="G93" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H93">
         <f>E93*VALUE(LEFT(G93, FIND(":", G93)-1))</f>
@@ -3577,21 +3869,21 @@
       </c>
     </row>
     <row r="94" spans="1:8">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1" t="s">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>264</v>
+      <c r="D94" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="E94">
         <v>0</v>
       </c>
       <c r="G94" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H94">
         <f>E94*VALUE(LEFT(G94, FIND(":", G94)-1))</f>
@@ -3599,19 +3891,19 @@
       </c>
     </row>
     <row r="95" spans="1:8">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1" t="s">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D95" s="2" t="s">
-        <v>265</v>
+      <c r="D95" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="E95">
         <v>0</v>
       </c>
       <c r="G95" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H95">
         <f>E95*VALUE(LEFT(G95, FIND(":", G95)-1))</f>
@@ -3619,19 +3911,19 @@
       </c>
     </row>
     <row r="96" spans="1:8">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1" t="s">
+      <c r="A96" s="2"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D96" s="2" t="s">
-        <v>266</v>
+      <c r="D96" s="3" t="s">
+        <v>267</v>
       </c>
       <c r="E96">
         <v>0</v>
       </c>
       <c r="G96" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H96">
         <f>E96*VALUE(LEFT(G96, FIND(":", G96)-1))</f>
@@ -3639,19 +3931,19 @@
       </c>
     </row>
     <row r="97" spans="1:8">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1" t="s">
+      <c r="A97" s="2"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>267</v>
+      <c r="D97" s="3" t="s">
+        <v>268</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
       <c r="G97" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H97">
         <f>E97*VALUE(LEFT(G97, FIND(":", G97)-1))</f>
@@ -3659,19 +3951,22 @@
       </c>
     </row>
     <row r="98" spans="1:8">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1" t="s">
+      <c r="A98" s="2"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>268</v>
+      <c r="D98" s="3" t="s">
+        <v>269</v>
       </c>
       <c r="E98">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>315</v>
       </c>
       <c r="G98" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H98">
         <f>E98*VALUE(LEFT(G98, FIND(":", G98)-1))</f>
@@ -3679,19 +3974,19 @@
       </c>
     </row>
     <row r="99" spans="1:8">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1" t="s">
+      <c r="A99" s="2"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D99" s="2" t="s">
-        <v>269</v>
+      <c r="D99" s="3" t="s">
+        <v>270</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99" t="s">
-        <v>308</v>
+        <v>362</v>
       </c>
       <c r="H99">
         <f>E99*VALUE(LEFT(G99, FIND(":", G99)-1))</f>
@@ -3699,19 +3994,19 @@
       </c>
     </row>
     <row r="100" spans="1:8">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1" t="s">
+      <c r="A100" s="2"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D100" s="2" t="s">
-        <v>270</v>
+      <c r="D100" s="3" t="s">
+        <v>271</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
       <c r="G100" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H100">
         <f>E100*VALUE(LEFT(G100, FIND(":", G100)-1))</f>
@@ -3719,21 +4014,24 @@
       </c>
     </row>
     <row r="101" spans="1:8">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1" t="s">
+      <c r="A101" s="2"/>
+      <c r="B101" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D101" s="2" t="s">
-        <v>271</v>
+      <c r="D101" s="3" t="s">
+        <v>272</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>316</v>
       </c>
       <c r="G101" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H101">
         <f>E101*VALUE(LEFT(G101, FIND(":", G101)-1))</f>
@@ -3741,19 +4039,19 @@
       </c>
     </row>
     <row r="102" spans="1:8">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1" t="s">
+      <c r="A102" s="2"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D102" s="2" t="s">
-        <v>272</v>
+      <c r="D102" s="3" t="s">
+        <v>273</v>
       </c>
       <c r="E102">
         <v>0</v>
       </c>
       <c r="G102" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H102">
         <f>E102*VALUE(LEFT(G102, FIND(":", G102)-1))</f>
@@ -3761,19 +4059,19 @@
       </c>
     </row>
     <row r="103" spans="1:8">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1" t="s">
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D103" s="2" t="s">
-        <v>273</v>
+      <c r="D103" s="3" t="s">
+        <v>274</v>
       </c>
       <c r="E103">
         <v>0</v>
       </c>
       <c r="G103" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H103">
         <f>E103*VALUE(LEFT(G103, FIND(":", G103)-1))</f>
@@ -3781,19 +4079,19 @@
       </c>
     </row>
     <row r="104" spans="1:8">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1" t="s">
+      <c r="A104" s="2"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D104" s="2" t="s">
-        <v>274</v>
+      <c r="D104" s="3" t="s">
+        <v>275</v>
       </c>
       <c r="E104">
         <v>0</v>
       </c>
       <c r="G104" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H104">
         <f>E104*VALUE(LEFT(G104, FIND(":", G104)-1))</f>
@@ -3801,19 +4099,19 @@
       </c>
     </row>
     <row r="105" spans="1:8">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1" t="s">
+      <c r="A105" s="2"/>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D105" s="2" t="s">
-        <v>275</v>
+      <c r="D105" s="3" t="s">
+        <v>276</v>
       </c>
       <c r="E105">
         <v>0</v>
       </c>
       <c r="G105" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H105">
         <f>E105*VALUE(LEFT(G105, FIND(":", G105)-1))</f>
@@ -3821,19 +4119,19 @@
       </c>
     </row>
     <row r="106" spans="1:8">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1" t="s">
+      <c r="A106" s="2"/>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D106" s="2" t="s">
-        <v>276</v>
+      <c r="D106" s="3" t="s">
+        <v>277</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G106" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H106">
         <f>E106*VALUE(LEFT(G106, FIND(":", G106)-1))</f>
@@ -3841,23 +4139,26 @@
       </c>
     </row>
     <row r="107" spans="1:8">
-      <c r="A107" s="1" t="s">
+      <c r="A107" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D107" s="2" t="s">
-        <v>277</v>
+      <c r="D107" s="3" t="s">
+        <v>278</v>
       </c>
       <c r="E107">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="G107" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H107">
         <f>E107*VALUE(LEFT(G107, FIND(":", G107)-1))</f>
@@ -3865,19 +4166,22 @@
       </c>
     </row>
     <row r="108" spans="1:8">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1" t="s">
+      <c r="A108" s="2"/>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D108" s="2" t="s">
-        <v>278</v>
+      <c r="D108" s="3" t="s">
+        <v>279</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>318</v>
       </c>
       <c r="G108" t="s">
-        <v>308</v>
+        <v>362</v>
       </c>
       <c r="H108">
         <f>E108*VALUE(LEFT(G108, FIND(":", G108)-1))</f>
@@ -3885,19 +4189,22 @@
       </c>
     </row>
     <row r="109" spans="1:8">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1" t="s">
+      <c r="A109" s="2"/>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D109" s="2" t="s">
-        <v>279</v>
+      <c r="D109" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>319</v>
       </c>
       <c r="G109" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H109">
         <f>E109*VALUE(LEFT(G109, FIND(":", G109)-1))</f>
@@ -3905,19 +4212,22 @@
       </c>
     </row>
     <row r="110" spans="1:8">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1" t="s">
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D110" s="2" t="s">
-        <v>280</v>
+      <c r="D110" s="3" t="s">
+        <v>281</v>
       </c>
       <c r="E110">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="G110" t="s">
-        <v>308</v>
+        <v>362</v>
       </c>
       <c r="H110">
         <f>E110*VALUE(LEFT(G110, FIND(":", G110)-1))</f>
@@ -3925,19 +4235,22 @@
       </c>
     </row>
     <row r="111" spans="1:8">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="1" t="s">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D111" s="2" t="s">
-        <v>281</v>
+      <c r="D111" s="3" t="s">
+        <v>282</v>
       </c>
       <c r="E111">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="G111" t="s">
-        <v>308</v>
+        <v>362</v>
       </c>
       <c r="H111">
         <f>E111*VALUE(LEFT(G111, FIND(":", G111)-1))</f>
@@ -3945,19 +4258,22 @@
       </c>
     </row>
     <row r="112" spans="1:8">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1" t="s">
+      <c r="A112" s="2"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D112" s="2" t="s">
-        <v>282</v>
+      <c r="D112" s="3" t="s">
+        <v>283</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="G112" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H112">
         <f>E112*VALUE(LEFT(G112, FIND(":", G112)-1))</f>
@@ -3965,19 +4281,19 @@
       </c>
     </row>
     <row r="113" spans="1:8">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="1" t="s">
+      <c r="A113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>283</v>
+      <c r="D113" s="3" t="s">
+        <v>284</v>
       </c>
       <c r="E113">
         <v>0</v>
       </c>
       <c r="G113" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H113">
         <f>E113*VALUE(LEFT(G113, FIND(":", G113)-1))</f>
@@ -3985,21 +4301,24 @@
       </c>
     </row>
     <row r="114" spans="1:8">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1" t="s">
+      <c r="A114" s="2"/>
+      <c r="B114" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D114" s="2" t="s">
-        <v>284</v>
+      <c r="D114" s="3" t="s">
+        <v>285</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="G114" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H114">
         <f>E114*VALUE(LEFT(G114, FIND(":", G114)-1))</f>
@@ -4007,19 +4326,22 @@
       </c>
     </row>
     <row r="115" spans="1:8">
-      <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1" t="s">
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D115" s="2" t="s">
-        <v>285</v>
+      <c r="D115" s="3" t="s">
+        <v>286</v>
       </c>
       <c r="E115">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="G115" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H115">
         <f>E115*VALUE(LEFT(G115, FIND(":", G115)-1))</f>
@@ -4027,19 +4349,19 @@
       </c>
     </row>
     <row r="116" spans="1:8">
-      <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1" t="s">
+      <c r="A116" s="2"/>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D116" s="2" t="s">
-        <v>286</v>
+      <c r="D116" s="3" t="s">
+        <v>287</v>
       </c>
       <c r="E116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G116" t="s">
-        <v>308</v>
+        <v>366</v>
       </c>
       <c r="H116">
         <f>E116*VALUE(LEFT(G116, FIND(":", G116)-1))</f>
@@ -4047,19 +4369,19 @@
       </c>
     </row>
     <row r="117" spans="1:8">
-      <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1" t="s">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D117" s="2" t="s">
-        <v>287</v>
+      <c r="D117" s="3" t="s">
+        <v>288</v>
       </c>
       <c r="E117">
         <v>0</v>
       </c>
       <c r="G117" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H117">
         <f>E117*VALUE(LEFT(G117, FIND(":", G117)-1))</f>
@@ -4067,19 +4389,19 @@
       </c>
     </row>
     <row r="118" spans="1:8">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1" t="s">
+      <c r="A118" s="2"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D118" s="2" t="s">
-        <v>288</v>
+      <c r="D118" s="3" t="s">
+        <v>289</v>
       </c>
       <c r="E118">
         <v>0</v>
       </c>
       <c r="G118" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H118">
         <f>E118*VALUE(LEFT(G118, FIND(":", G118)-1))</f>
@@ -4087,19 +4409,22 @@
       </c>
     </row>
     <row r="119" spans="1:8">
-      <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1" t="s">
+      <c r="A119" s="2"/>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>289</v>
+      <c r="D119" s="3" t="s">
+        <v>290</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="G119" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H119">
         <f>E119*VALUE(LEFT(G119, FIND(":", G119)-1))</f>
@@ -4107,19 +4432,19 @@
       </c>
     </row>
     <row r="120" spans="1:8">
-      <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
-      <c r="C120" s="1" t="s">
+      <c r="A120" s="2"/>
+      <c r="B120" s="2"/>
+      <c r="C120" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D120" s="2" t="s">
-        <v>290</v>
+      <c r="D120" s="3" t="s">
+        <v>291</v>
       </c>
       <c r="E120">
         <v>0</v>
       </c>
       <c r="G120" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H120">
         <f>E120*VALUE(LEFT(G120, FIND(":", G120)-1))</f>
@@ -4127,21 +4452,21 @@
       </c>
     </row>
     <row r="121" spans="1:8">
-      <c r="A121" s="1"/>
-      <c r="B121" s="1" t="s">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D121" s="2" t="s">
-        <v>291</v>
+      <c r="D121" s="3" t="s">
+        <v>292</v>
       </c>
       <c r="E121">
         <v>0</v>
       </c>
       <c r="G121" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H121">
         <f>E121*VALUE(LEFT(G121, FIND(":", G121)-1))</f>
@@ -4149,19 +4474,19 @@
       </c>
     </row>
     <row r="122" spans="1:8">
-      <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1" t="s">
+      <c r="A122" s="2"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D122" s="2" t="s">
-        <v>292</v>
+      <c r="D122" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="E122">
         <v>0</v>
       </c>
       <c r="G122" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H122">
         <f>E122*VALUE(LEFT(G122, FIND(":", G122)-1))</f>
@@ -4169,19 +4494,19 @@
       </c>
     </row>
     <row r="123" spans="1:8">
-      <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1" t="s">
+      <c r="A123" s="2"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D123" s="2" t="s">
-        <v>293</v>
+      <c r="D123" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="E123">
         <v>0</v>
       </c>
       <c r="G123" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H123">
         <f>E123*VALUE(LEFT(G123, FIND(":", G123)-1))</f>
@@ -4189,19 +4514,19 @@
       </c>
     </row>
     <row r="124" spans="1:8">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-      <c r="C124" s="1" t="s">
+      <c r="A124" s="2"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D124" s="2" t="s">
-        <v>294</v>
+      <c r="D124" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="E124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G124" t="s">
-        <v>308</v>
+        <v>367</v>
       </c>
       <c r="H124">
         <f>E124*VALUE(LEFT(G124, FIND(":", G124)-1))</f>
@@ -4209,19 +4534,19 @@
       </c>
     </row>
     <row r="125" spans="1:8">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
-      <c r="C125" s="1" t="s">
+      <c r="A125" s="2"/>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D125" s="2" t="s">
-        <v>295</v>
+      <c r="D125" s="3" t="s">
+        <v>296</v>
       </c>
       <c r="E125">
         <v>0</v>
       </c>
       <c r="G125" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H125">
         <f>E125*VALUE(LEFT(G125, FIND(":", G125)-1))</f>
@@ -4229,19 +4554,22 @@
       </c>
     </row>
     <row r="126" spans="1:8">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
-      <c r="C126" s="1" t="s">
+      <c r="A126" s="2"/>
+      <c r="B126" s="2"/>
+      <c r="C126" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D126" s="2" t="s">
-        <v>296</v>
+      <c r="D126" s="3" t="s">
+        <v>297</v>
       </c>
       <c r="E126">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="G126" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H126">
         <f>E126*VALUE(LEFT(G126, FIND(":", G126)-1))</f>
@@ -4249,19 +4577,22 @@
       </c>
     </row>
     <row r="127" spans="1:8">
-      <c r="A127" s="1"/>
-      <c r="B127" s="1"/>
-      <c r="C127" s="1" t="s">
+      <c r="A127" s="2"/>
+      <c r="B127" s="2"/>
+      <c r="C127" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D127" s="2" t="s">
-        <v>297</v>
+      <c r="D127" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="E127">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="G127" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H127">
         <f>E127*VALUE(LEFT(G127, FIND(":", G127)-1))</f>
@@ -4269,19 +4600,19 @@
       </c>
     </row>
     <row r="128" spans="1:8">
-      <c r="A128" s="1"/>
-      <c r="B128" s="1"/>
-      <c r="C128" s="1" t="s">
+      <c r="A128" s="2"/>
+      <c r="B128" s="2"/>
+      <c r="C128" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D128" s="2" t="s">
-        <v>298</v>
+      <c r="D128" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="E128">
         <v>0</v>
       </c>
       <c r="G128" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H128">
         <f>E128*VALUE(LEFT(G128, FIND(":", G128)-1))</f>
@@ -4289,21 +4620,19 @@
       </c>
     </row>
     <row r="129" spans="1:8">
-      <c r="A129" s="1"/>
-      <c r="B129" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C129" s="1" t="s">
+      <c r="A129" s="2"/>
+      <c r="B129" s="2"/>
+      <c r="C129" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D129" s="2" t="s">
-        <v>299</v>
+      <c r="D129" s="3" t="s">
+        <v>295</v>
       </c>
       <c r="E129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G129" t="s">
-        <v>308</v>
+        <v>367</v>
       </c>
       <c r="H129">
         <f>E129*VALUE(LEFT(G129, FIND(":", G129)-1))</f>
@@ -4311,19 +4640,21 @@
       </c>
     </row>
     <row r="130" spans="1:8">
-      <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1" t="s">
+      <c r="A130" s="2"/>
+      <c r="B130" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="D130" s="2" t="s">
+      <c r="D130" s="3" t="s">
         <v>300</v>
       </c>
       <c r="E130">
         <v>0</v>
       </c>
       <c r="G130" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H130">
         <f>E130*VALUE(LEFT(G130, FIND(":", G130)-1))</f>
@@ -4331,19 +4662,22 @@
       </c>
     </row>
     <row r="131" spans="1:8">
-      <c r="A131" s="1"/>
-      <c r="B131" s="1"/>
-      <c r="C131" s="1" t="s">
+      <c r="A131" s="2"/>
+      <c r="B131" s="2"/>
+      <c r="C131" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D131" s="2" t="s">
+      <c r="D131" s="3" t="s">
         <v>301</v>
       </c>
       <c r="E131">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>328</v>
       </c>
       <c r="G131" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H131">
         <f>E131*VALUE(LEFT(G131, FIND(":", G131)-1))</f>
@@ -4351,19 +4685,22 @@
       </c>
     </row>
     <row r="132" spans="1:8">
-      <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
-      <c r="C132" s="1" t="s">
+      <c r="A132" s="2"/>
+      <c r="B132" s="2"/>
+      <c r="C132" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D132" s="2" t="s">
+      <c r="D132" s="3" t="s">
         <v>302</v>
       </c>
       <c r="E132">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="G132" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
       <c r="H132">
         <f>E132*VALUE(LEFT(G132, FIND(":", G132)-1))</f>
@@ -4371,19 +4708,19 @@
       </c>
     </row>
     <row r="133" spans="1:8">
-      <c r="A133" s="1"/>
-      <c r="B133" s="1"/>
-      <c r="C133" s="1" t="s">
+      <c r="A133" s="2"/>
+      <c r="B133" s="2"/>
+      <c r="C133" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D133" s="2" t="s">
+      <c r="D133" s="3" t="s">
         <v>303</v>
       </c>
       <c r="E133">
         <v>0</v>
       </c>
       <c r="G133" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H133">
         <f>E133*VALUE(LEFT(G133, FIND(":", G133)-1))</f>
@@ -4391,19 +4728,19 @@
       </c>
     </row>
     <row r="134" spans="1:8">
-      <c r="A134" s="1"/>
-      <c r="B134" s="1"/>
-      <c r="C134" s="1" t="s">
+      <c r="A134" s="2"/>
+      <c r="B134" s="2"/>
+      <c r="C134" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D134" s="2" t="s">
+      <c r="D134" s="3" t="s">
         <v>304</v>
       </c>
       <c r="E134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G134" t="s">
-        <v>308</v>
+        <v>366</v>
       </c>
       <c r="H134">
         <f>E134*VALUE(LEFT(G134, FIND(":", G134)-1))</f>
@@ -4411,22 +4748,42 @@
       </c>
     </row>
     <row r="135" spans="1:8">
-      <c r="A135" s="1"/>
-      <c r="B135" s="1"/>
-      <c r="C135" s="1" t="s">
+      <c r="A135" s="2"/>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D135" s="2" t="s">
+      <c r="D135" s="3" t="s">
         <v>305</v>
       </c>
       <c r="E135">
         <v>0</v>
       </c>
       <c r="G135" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="H135">
         <f>E135*VALUE(LEFT(G135, FIND(":", G135)-1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
+      <c r="A136" s="2"/>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="G136" t="s">
+        <v>355</v>
+      </c>
+      <c r="H136">
+        <f>E136*VALUE(LEFT(G136, FIND(":", G136)-1))</f>
         <v>0</v>
       </c>
     </row>
@@ -4435,7 +4792,7 @@
     <mergeCell ref="A2:A45"/>
     <mergeCell ref="A46:A75"/>
     <mergeCell ref="A76:A106"/>
-    <mergeCell ref="A107:A135"/>
+    <mergeCell ref="A107:A136"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="B12:B16"/>
@@ -4456,10 +4813,10 @@
     <mergeCell ref="B101:B106"/>
     <mergeCell ref="B107:B113"/>
     <mergeCell ref="B114:B120"/>
-    <mergeCell ref="B121:B128"/>
-    <mergeCell ref="B129:B135"/>
+    <mergeCell ref="B121:B129"/>
+    <mergeCell ref="B130:B136"/>
   </mergeCells>
-  <dataValidations count="134">
+  <dataValidations count="135">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
       <formula1>"0: None"</formula1>
     </dataValidation>
@@ -4470,13 +4827,13 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Not monitored,2: Reported,5: Manual remediation,10: Automated remediation"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6">
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7">
-      <formula1>"1: Test for 1,5: Test for 5,10: Test for 10"</formula1>
+      <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8">
       <formula1>"0: None"</formula1>
@@ -4500,13 +4857,13 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,5: 1 item completed,10: 2 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G16">
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G17">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Not done,10: Defined"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G18">
       <formula1>"0: None"</formula1>
@@ -4527,13 +4884,13 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G24">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No rules established,10: Published policy"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G25">
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G26">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,2: 1 item completed,4: 2 items completed,6: 3 items completed,8: 4 items completed,10: 5 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G27">
       <formula1>"0: None"</formula1>
@@ -4563,7 +4920,7 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G36">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Not done,10: Done and clealy defined"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G37">
       <formula1>"0: None"</formula1>
@@ -4572,7 +4929,7 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G39">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Not done,10: Defined"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G40">
       <formula1>"0: None"</formula1>
@@ -4581,7 +4938,7 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G42">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,4: 1 item completed,7: 2 items completed,10: 3 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G43">
       <formula1>"0: None"</formula1>
@@ -4593,13 +4950,13 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G46">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Does not exist,10: Exists"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G47">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,2: 1 item completed,4: 2 items completed,6: 3 items completed,8: 4 items completed,10: 5 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G48">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No documented method,10: Documented method of assessing modernization efforts"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G49">
       <formula1>"0: None"</formula1>
@@ -4629,7 +4986,7 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G58">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: 0%,1: 10%,2: 20%,3: 30%,4: 40%,5: 50%,6: 60%,7: 70%,8: 80%,9: 90%,10: Near 100%"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G59">
       <formula1>"0: None"</formula1>
@@ -4638,7 +4995,7 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G61">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Not done,10: Policy in place and published"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G62">
       <formula1>"0: None"</formula1>
@@ -4647,10 +5004,10 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G64">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Not done,10: Policy in place and published"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G65">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Not done,10: Policy in place and published"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G66">
       <formula1>"0: None"</formula1>
@@ -4662,16 +5019,16 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G69">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,2: 1 item completed,4: 2 items completed,6: 3 items completed,8: 4 items completed,10: 5 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G70">
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G71">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No teardown/shutdown policy,3: Published policy,6: Classification tagged or otherwise identifiable,10: Enforced Policy with tagged/identifiable classifications"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G72">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: 0%,1: 10%,2: 20%,3: 30%,4: 40%,5: 50%,6: 60%,7: 70%,8: 80%,9: 90%,10: Near 100%"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G73">
       <formula1>"0: None"</formula1>
@@ -4695,16 +5052,16 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G80">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No review of trends,3: Manual review of trends,6: Automated trend detection,10: Manual review and automated trend detection"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G81">
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G82">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Does not exist,10: Exists"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G83">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Does not exist,10: Exists"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G84">
       <formula1>"0: None"</formula1>
@@ -4722,19 +5079,19 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G89">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,3: 1 item completed,5: 2 items completed,8: 3 items completed,10: 4 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G90">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: None,1: Annual,2: Quarterly,5: Monthly,7: Bi-Weekly,8: Weekly,10: Daily"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G91">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: 0%,1: 10%,2: 20%,3: 30%,4: 40%,5: 50%,6: 60%,7: 70%,8: 80%,9: 90%,10: Near 100%"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G92">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No alerting,10: Alerting exists"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G93">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,3: 1 item completed,5: 2 items completed,8: 3 items completed,10: 4 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G94">
       <formula1>"0: None"</formula1>
@@ -4749,16 +5106,16 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G98">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,4: 1 item completed,7: 2 items completed,10: 3 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G99">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: 0%,1: 10%,2: 20%,3: 30%,4: 40%,5: 50%,6: 60%,7: 70%,8: 80%,9: 90%,10: Near 100%"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G100">
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G101">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,3: 1 item completed,5: 2 items completed,8: 3 items completed,10: 4 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G102">
       <formula1>"0: None"</formula1>
@@ -4773,37 +5130,37 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G106">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: None,10: set goal thresholds for kpis and unit costs"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G107">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,5: 1 item completed,10: 2 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G108">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: 0%,1: 10%,2: 20%,3: 30%,4: 40%,5: 50%,6: 60%,7: 70%,8: 80% ,9: 90%,10: Near 100%"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G109">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,5: 1 item  completed,10: 2 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G110">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: 0%,1: 10%,2: 20%,3: 30%,4: 40%,5: 50%,6: 60%,7: 70%,8: 80%,9: 90%,10: Near 100%"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G111">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: 0%,1: 10%,2: 20%,3: 30%,4: 40%,5: 50%,6: 60%,7: 70%,8: 80%,9: 90%,10: Near 100%"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G112">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,3: 1 item completed,5: 2 items completed,8: 3 items completed,10: 4 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G113">
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G114">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,2: 1 item completed,4: 2 items completed,6: 3 items completed,8: 4 items completed,10: 5 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G115">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,2: 1 item completed,4: 2 items completed,5: 3 items completed,7: 4 items completed,9: 5 items completed,10: 6 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G116">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No alerting in worflow tools,1: Alerting in at least one tool,3: Alerting in some tooling [20%],6: Alerting in most tooling [60%],10: Alerting in all workflow tools [100%]"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G117">
       <formula1>"0: None"</formula1>
@@ -4812,7 +5169,7 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G119">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,2: 1 item completed,3: 2 items completed,4: 3 items completed,5: 4 items completed,7: 5 items completed,8: 6 items completed,9: 7 items completed,10: 8 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G120">
       <formula1>"0: None"</formula1>
@@ -4827,39 +5184,42 @@
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G124">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Never,1: Monthly or greater,2: More than a week,3: 7 days,4: 5 days,6: 2 days,8: 1 day,10: Instant"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G125">
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G126">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,2: 1 items completed,3: 2 items completed,5: 3 items completed,6: 4 items completed,8: 5 items completed,9: 6 items completed,10: 7 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G127">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,2: 1 items completed,3: 2 items completed,5: 3 items completed,6: 4 items completed,8: 5 items completed,9: 6 items completed,10: 7 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G128">
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G129">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: Never,1: Monthly or greater,2: More than a week,3: 7 days,4: 5 days,6: 2 days,8: 1 day,10: Instant"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G130">
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G131">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,3: 1 item completed,5: 2 items completed,8: 3 items completed,10: 4 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G132">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No items completed,3: 1 item completed,5: 2 items completed,8: 3 items completed,10: 4 items completed"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G133">
       <formula1>"0: None"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G134">
-      <formula1>"0: None"</formula1>
+      <formula1>"0: No alerting in worflow tools,1: Alerting in at least one tool,3: Alerting in some tooling [20%],6: Alerting in most tooling [60%],10: Alerting in all workflow tools [100%]"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G135">
+      <formula1>"0: None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G136">
       <formula1>"0: None"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4998,6 +5358,7 @@
     <hyperlink ref="D133" r:id="rId132"/>
     <hyperlink ref="D134" r:id="rId133"/>
     <hyperlink ref="D135" r:id="rId134"/>
+    <hyperlink ref="D136" r:id="rId135"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>